<commit_message>
Moved some configuration settings to config and added support for multiple sequence passes
</commit_message>
<xml_diff>
--- a/WebAuto.Tests/TestFiles/Data/Test Search 1.xlsx
+++ b/WebAuto.Tests/TestFiles/Data/Test Search 1.xlsx
@@ -9,15 +9,16 @@
   <sheets>
     <sheet name="GotoSearchPage" sheetId="1" r:id="rId1"/>
     <sheet name="NormalSearch" sheetId="4" r:id="rId2"/>
-    <sheet name="FeelingLuckySearch" sheetId="5" r:id="rId3"/>
-    <sheet name="FollowFirstResult" sheetId="6" r:id="rId4"/>
+    <sheet name="NormalSearch(2)" sheetId="7" r:id="rId3"/>
+    <sheet name="FeelingLuckySearch" sheetId="5" r:id="rId4"/>
+    <sheet name="FollowFirstResult" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Key</t>
   </si>
@@ -53,6 +54,18 @@
   </si>
   <si>
     <t>vegetables</t>
+  </si>
+  <si>
+    <t>companies</t>
+  </si>
+  <si>
+    <t>televisions</t>
+  </si>
+  <si>
+    <t>ninjas</t>
+  </si>
+  <si>
+    <t>im feeling lucky</t>
   </si>
 </sst>
 </file>
@@ -451,7 +464,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,14 +502,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
@@ -507,18 +558,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -526,11 +569,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>

</xml_diff>